<commit_message>
alterações Tabela de Requisitos
</commit_message>
<xml_diff>
--- a/doc/team-requisitos/Tabela de Requisitos.xlsx
+++ b/doc/team-requisitos/Tabela de Requisitos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Catarina Pires\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DDBDBCB1-FB59-460B-8C5D-A2B8B0335908}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{74922CD8-1B71-4A93-9D7E-0CC1860967F0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="47">
   <si>
     <t>Requisito</t>
   </si>
@@ -55,10 +55,6 @@
     <t>Alterado</t>
   </si>
   <si>
-    <t>O utilizador tem de usar os seus dados pessoais para se
- registar na app</t>
-  </si>
-  <si>
     <t>1º Sprint</t>
   </si>
   <si>
@@ -69,9 +65,6 @@
   </si>
   <si>
     <t>No ato de registo, verificar que o ORCID inserido é válido</t>
-  </si>
-  <si>
-    <t>O utilizador tem de poder efetuar o login e logout</t>
   </si>
   <si>
     <t>Média</t>
@@ -81,17 +74,7 @@
 várias opções de navegação pela app</t>
   </si>
   <si>
-    <t>O utilizador pode aceder ao seu perfil</t>
-  </si>
-  <si>
     <t>O utilizador pode aceder ao perfil de outro utilizador</t>
-  </si>
-  <si>
-    <t>Performance: não demorar mais de 2 segundos a carregar
-páginas</t>
-  </si>
-  <si>
-    <t>O utilizador pode repor a sua password caso se esqueça</t>
   </si>
   <si>
     <t>O utilizador pode publicar uma notícia no feed</t>
@@ -210,15 +193,80 @@
     <t>LEGENDA</t>
   </si>
   <si>
-    <t>Efetuado o login com sucesso a app mostra um feed de notícias de 
-acordo com as preferências do utilizador</t>
+    <t>O utilizador deve introduzir a sua data de nascimento no Registo</t>
+  </si>
+  <si>
+    <t>O utilizador tem de fornecer o primeiro e último nome no Registo</t>
+  </si>
+  <si>
+    <t>O utilizador deve introduzir uma instituição à qual está filiado.</t>
+  </si>
+  <si>
+    <t>O utilizador pode associar-se a uma ou mais Research Units</t>
+  </si>
+  <si>
+    <t>No registo, o utilizador cria um username e password.</t>
+  </si>
+  <si>
+    <t>O utilizador deve poder selecionar (escrever) os seus temas.</t>
+  </si>
+  <si>
+    <t>O utilizador deve poder cancelar o processo de registo a qualquer momento.</t>
+  </si>
+  <si>
+    <t>No login deve ser sugerida a recuperação de password a um utilizador que erre a palavra-passe mais que 3 vezes</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>Após o registo, o utilizador é redirecionado para o feed.</t>
+  </si>
+  <si>
+    <t>O utilizador pode efetuar logout</t>
+  </si>
+  <si>
+    <t>Se os dados de login estiverem corretos, o utilizador é redirecionado para o feed de notícias</t>
+  </si>
+  <si>
+    <t>O feed de notícias tem de estar de acordo com as preferências do utilizador</t>
+  </si>
+  <si>
+    <t>Em cada ecrã o botão “?” deve fornecer informação relevante à navegação do utilizador.</t>
+  </si>
+  <si>
+    <t>Cada post apresenta foto e nome de quem postou, assim como o conteúdo</t>
+  </si>
+  <si>
+    <t>No registo o utilizador insere um email válido</t>
+  </si>
+  <si>
+    <t>O utilizador consegue aceder ao seu perfil através do feed</t>
+  </si>
+  <si>
+    <t>No registo devem ser sugeridos temas de interesse populares ao utilizador</t>
+  </si>
+  <si>
+    <t>O utilizador deve ser capaz de selecionar temas de interesse sugeridos pela aplicação</t>
+  </si>
+  <si>
+    <t>Performance: não demorar mais de 3 segundos a carregar páginas</t>
+  </si>
+  <si>
+    <t>O perfil do utilizador contém: O seu nome, research unit(s), instituição, temas de interesse e uma fotografia</t>
+  </si>
+  <si>
+    <t>Estando no seu perfil, pode retroceder para a página do feed</t>
+  </si>
+  <si>
+    <t>Não</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -237,17 +285,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -338,7 +375,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -347,53 +384,38 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -402,41 +424,22 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -447,141 +450,86 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -900,10 +848,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:L22"/>
+  <dimension ref="B2:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -920,305 +868,650 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="B3" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="7">
+    <row r="3" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="9">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+    </row>
+    <row r="4" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="11"/>
-    </row>
-    <row r="4" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="12" t="s">
+      <c r="C4" s="9">
+        <v>2</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="13">
-        <v>2</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="13" t="s">
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+    </row>
+    <row r="5" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="25">
+        <v>3</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+    </row>
+    <row r="6" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="25">
+        <v>4</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+    </row>
+    <row r="7" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="25">
+        <v>5</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+    </row>
+    <row r="8" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="25">
+        <v>6</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+    </row>
+    <row r="9" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B9" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="25">
+        <v>7</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+    </row>
+    <row r="10" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="25">
+        <v>8</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+    </row>
+    <row r="11" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="25">
+        <v>9</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+    </row>
+    <row r="12" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="25">
+        <v>10</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+    </row>
+    <row r="13" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="25">
+        <v>11</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+    </row>
+    <row r="14" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="25">
+        <v>12</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+    </row>
+    <row r="15" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="25">
+        <v>13</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+    </row>
+    <row r="16" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="25">
         <v>14</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="17"/>
-    </row>
-    <row r="5" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="12" t="s">
+      <c r="D16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+    </row>
+    <row r="17" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="9">
+        <v>15</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+    </row>
+    <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="9">
         <v>16</v>
       </c>
-      <c r="C5" s="13">
-        <v>3</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="13" t="s">
+      <c r="D18" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="17"/>
-    </row>
-    <row r="6" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B6" s="12" t="s">
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+    </row>
+    <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="9">
+        <v>17</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+    </row>
+    <row r="20" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="9">
+        <v>18</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+    </row>
+    <row r="21" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="9">
+        <v>19</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+    </row>
+    <row r="22" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="9">
+        <v>20</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+    </row>
+    <row r="23" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="9">
+        <v>21</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+    </row>
+    <row r="24" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="9">
         <v>22</v>
       </c>
-      <c r="C6" s="13">
-        <v>4</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="13" t="s">
+      <c r="D24" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="17"/>
-    </row>
-    <row r="7" spans="2:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="B7" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="13">
-        <v>5</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="13" t="s">
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+    </row>
+    <row r="25" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="9">
+        <v>23</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="17"/>
-    </row>
-    <row r="8" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B8" s="12" t="s">
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+    </row>
+    <row r="26" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="13">
-        <v>6</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="13" t="s">
+      <c r="C26" s="9">
+        <v>24</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="17"/>
-    </row>
-    <row r="9" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="12" t="s">
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+    </row>
+    <row r="27" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="9">
+        <v>25</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+    </row>
+    <row r="28" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H29" s="1"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="13">
-        <v>7</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="17"/>
-    </row>
-    <row r="10" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10" s="12" t="s">
+    </row>
+    <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="13">
-        <v>8</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="17"/>
-    </row>
-    <row r="11" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="13">
-        <v>9</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="17"/>
-    </row>
-    <row r="12" spans="2:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="B12" s="28" t="s">
+    </row>
+    <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="19">
-        <v>10</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="23"/>
-    </row>
-    <row r="15" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H16" s="1"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="25"/>
-    </row>
-    <row r="19" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="25" t="s">
-        <v>27</v>
+    </row>
+    <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>